<commit_message>
- Added data driven concepts--> Reading data from excel,retry analyzer, AnnotationTransformer, selenoid configuration etc
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,39 +21,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i</t>
-  </si>
-  <si>
-    <t xml:space="preserve">love</t>
-  </si>
-  <si>
-    <t xml:space="preserve">you</t>
-  </si>
-  <si>
-    <t xml:space="preserve">are</t>
-  </si>
-  <si>
-    <t xml:space="preserve">my</t>
-  </si>
-  <si>
-    <t xml:space="preserve">everything</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">testname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testdescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">execute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginorm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chromegrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safari</t>
   </si>
 </sst>
 </file>
@@ -62,11 +84,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,6 +105,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,8 +154,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,54 +294,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.94"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -313,4 +347,113 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Exception Handling -Java Doc -Code Optimization -Docker compose -Etc
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
@@ -38,18 +38,24 @@
     <t xml:space="preserve">first test case</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loginorm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second test case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testAmazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demo amazon</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">loginorm1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">second test case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">browser</t>
   </si>
   <si>
@@ -59,6 +65,9 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">menutext</t>
+  </si>
+  <si>
     <t xml:space="preserve">chromegrid</t>
   </si>
   <si>
@@ -75,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">safari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Sellers</t>
   </si>
 </sst>
 </file>
@@ -84,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,11 +117,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +161,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,10 +171,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,10 +297,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -335,7 +338,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -354,10 +368,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -370,13 +384,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,14 +403,17 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,15 +421,18 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -421,13 +444,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,16 +461,39 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Cucumber, -github result
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" state="visible" r:id="rId3"/>
@@ -299,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C6 D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -370,8 +370,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,7 +484,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
local chrome with headless
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -68,19 +68,19 @@
     <t xml:space="preserve">menutext</t>
   </si>
   <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin124</t>
+  </si>
+  <si>
     <t xml:space="preserve">chromegrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin124</t>
   </si>
   <si>
     <t xml:space="preserve">safari</t>
@@ -300,7 +300,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="C2 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,7 +371,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,13 +424,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
@@ -444,7 +444,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -470,7 +470,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
@@ -484,13 +484,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
working on the github action to make work
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -68,19 +68,19 @@
     <t xml:space="preserve">menutext</t>
   </si>
   <si>
+    <t xml:space="preserve">chromegrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin123</t>
-  </si>
-  <si>
     <t xml:space="preserve">admin124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chromegrid</t>
   </si>
   <si>
     <t xml:space="preserve">safari</t>
@@ -424,13 +424,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
@@ -444,7 +444,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -470,7 +470,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
@@ -484,13 +484,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
-Log4j-Basics -Owner Library -highlight -Code Checkstyle Maven plugin
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" state="visible" r:id="rId3"/>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">admin123</t>
   </si>
   <si>
+    <t xml:space="preserve">admin124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safari</t>
+  </si>
+  <si>
     <t xml:space="preserve">chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">safari</t>
   </si>
   <si>
     <t xml:space="preserve">Best Sellers</t>
@@ -299,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="C2 D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -370,8 +370,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,13 +424,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
@@ -464,13 +464,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
@@ -484,13 +484,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
- Appium browser execution successfully implemented
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
@@ -68,13 +68,16 @@
     <t xml:space="preserve">menutext</t>
   </si>
   <si>
+    <t xml:space="preserve">android</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
     <t xml:space="preserve">chromegrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin123</t>
   </si>
   <si>
     <t xml:space="preserve">admin124</t>
@@ -299,7 +302,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -370,8 +373,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,13 +427,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
@@ -444,7 +447,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -464,13 +467,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
@@ -484,16 +487,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before api code (#3)
* Dev Tools Code Added

* Dev Tools Code Added

* Dev Tools Code Added

* Started working on the DB Testing

* using  javassist Dynamic Pojo Class created successfully.

* Selenium-Gird TOML Configuration File

* API Started
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -68,16 +68,16 @@
     <t xml:space="preserve">menutext</t>
   </si>
   <si>
+    <t xml:space="preserve">chromegrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
     <t xml:space="preserve">android</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chromegrid</t>
   </si>
   <si>
     <t xml:space="preserve">admin124</t>
@@ -374,7 +374,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,7 +447,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>

</xml_diff>